<commit_message>
P230 preferred names and changes
</commit_message>
<xml_diff>
--- a/studentList_P230.xlsx
+++ b/studentList_P230.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/git/pub/makeSmallGroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DF3F15-4B37-FE40-BDE4-2E4B7C4F149D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776414E0-1836-6048-BD64-9D4902807B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="500" windowWidth="27260" windowHeight="16940" xr2:uid="{8A4E183B-1811-A24F-B56A-03E1FE378DEE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="70">
   <si>
     <t>ANTICH, JOVAN</t>
   </si>
@@ -198,9 +198,6 @@
     <t>Brady</t>
   </si>
   <si>
-    <t>Dayeon</t>
-  </si>
-  <si>
     <t>Lorenzo</t>
   </si>
   <si>
@@ -238,6 +235,15 @@
   </si>
   <si>
     <t>Students</t>
+  </si>
+  <si>
+    <t>Yeon</t>
+  </si>
+  <si>
+    <t>Nora</t>
+  </si>
+  <si>
+    <t>Allen</t>
   </si>
 </sst>
 </file>
@@ -607,9 +613,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB30F65-A83E-A445-BF53-0C354A2986B1}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -619,7 +627,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -693,7 +701,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="1">
         <v>80739182</v>
@@ -785,7 +793,7 @@
     </row>
     <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="B9" s="1">
         <v>59646361</v>
@@ -808,7 +816,7 @@
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="1">
         <v>40962920</v>
@@ -831,7 +839,7 @@
     </row>
     <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="1">
         <v>95807783</v>
@@ -854,7 +862,7 @@
     </row>
     <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" s="1">
         <v>45568300</v>
@@ -877,7 +885,7 @@
     </row>
     <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B13" s="1">
         <v>92924601</v>
@@ -900,7 +908,7 @@
     </row>
     <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="1">
         <v>17286660</v>
@@ -923,7 +931,7 @@
     </row>
     <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="1">
         <v>88366039</v>
@@ -946,7 +954,7 @@
     </row>
     <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="1">
         <v>39566479</v>
@@ -969,7 +977,7 @@
     </row>
     <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" s="1">
         <v>78682273</v>
@@ -992,7 +1000,7 @@
     </row>
     <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" s="1">
         <v>61366112</v>
@@ -1015,7 +1023,7 @@
     </row>
     <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" s="1">
         <v>39646529</v>
@@ -1038,7 +1046,7 @@
     </row>
     <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B20" s="1">
         <v>64603961</v>
@@ -1057,6 +1065,16 @@
       </c>
       <c r="G20" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
larger class sizes ugh
</commit_message>
<xml_diff>
--- a/studentList_P230.xlsx
+++ b/studentList_P230.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/git/pub/makeSmallGroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C9814A-9E26-7E47-A991-26B271D32BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314F5A88-66D0-0043-A452-E10EABDBF2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12240" yWindow="8360" windowWidth="27260" windowHeight="16940" xr2:uid="{8A4E183B-1811-A24F-B56A-03E1FE378DEE}"/>
+    <workbookView xWindow="1540" yWindow="1060" windowWidth="27260" windowHeight="16940" xr2:uid="{8A4E183B-1811-A24F-B56A-03E1FE378DEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="66">
   <si>
     <t>ANTICH, JOVAN</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>Natalie</t>
+  </si>
+  <si>
+    <t>Lorenzo</t>
   </si>
 </sst>
 </file>
@@ -605,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB30F65-A83E-A445-BF53-0C354A2986B1}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1026,6 +1029,11 @@
     <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upgrade to work with newest versions of packages
</commit_message>
<xml_diff>
--- a/studentList_P230.xlsx
+++ b/studentList_P230.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/git/pub/makeSmallGroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CA1419-541A-EB41-9758-476D2B0F1C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4351473-D55C-CF41-8DE0-A9ECBC818183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34980" yWindow="1160" windowWidth="27260" windowHeight="16940" xr2:uid="{8A4E183B-1811-A24F-B56A-03E1FE378DEE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Students</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>Justin</t>
-  </si>
-  <si>
-    <t>Vincent</t>
   </si>
   <si>
     <t>Teddy</t>
@@ -504,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB30F65-A83E-A445-BF53-0C354A2986B1}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -720,7 +717,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -741,11 +738,6 @@
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update for fall 2024
</commit_message>
<xml_diff>
--- a/studentList_P230.xlsx
+++ b/studentList_P230.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/git/pub/makeSmallGroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4351473-D55C-CF41-8DE0-A9ECBC818183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F3D0ED-3A26-4B43-B1AE-7B5DE0C8F7CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34980" yWindow="1160" windowWidth="27260" windowHeight="16940" xr2:uid="{8A4E183B-1811-A24F-B56A-03E1FE378DEE}"/>
   </bookViews>
@@ -34,97 +34,166 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
   <si>
     <t>Students</t>
   </si>
   <si>
-    <t>39206400        AGERBO, GUSTAV NORGAARD GAGERBO@UCI.EDU PHYSICS SR      GR</t>
-  </si>
-  <si>
-    <t>66099185        DROBNY, MACKENZIE ELIZABETH     MDROBNY@UCI.EDU PHYSICS SR      GR</t>
-  </si>
-  <si>
-    <t>24417898        SHI, JINGCHENG  JINGCS2@UCI.EDU PHYSICS SR      GR</t>
-  </si>
-  <si>
-    <t>54951864        WU, NICHOLAS YI JUN     NYWU1@UCI.EDU   PHYSICS SR      GR</t>
-  </si>
-  <si>
-    <t>80412038        ZHANG, SHAOHENG SHAOHEZ1@UCI.EDU        PHYSICS SR      GR</t>
-  </si>
-  <si>
-    <t>Caroline</t>
-  </si>
-  <si>
-    <t>Abbey</t>
-  </si>
-  <si>
-    <t>Arvind</t>
-  </si>
-  <si>
-    <t>Ren</t>
-  </si>
-  <si>
-    <t>Austin</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Dylan</t>
-  </si>
-  <si>
-    <t>Kyla</t>
-  </si>
-  <si>
-    <t>Luke</t>
-  </si>
-  <si>
-    <t>Luis</t>
-  </si>
-  <si>
-    <t>Madison</t>
-  </si>
-  <si>
-    <t>Rany</t>
-  </si>
-  <si>
-    <t>Yonghan</t>
-  </si>
-  <si>
-    <t>Qingyuan</t>
-  </si>
-  <si>
-    <t>Zhishun</t>
-  </si>
-  <si>
-    <t>Jacy</t>
-  </si>
-  <si>
-    <t>Gustav</t>
-  </si>
-  <si>
-    <t>Jingcheng</t>
-  </si>
-  <si>
-    <t>Nicholas</t>
-  </si>
-  <si>
-    <t>Shaoheng</t>
-  </si>
-  <si>
-    <t>Justin</t>
-  </si>
-  <si>
-    <t>Teddy</t>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>Kate</t>
+  </si>
+  <si>
+    <t>Student#</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>Lvl</t>
+  </si>
+  <si>
+    <t>Opt</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>BOADA, PATRICK</t>
+  </si>
+  <si>
+    <t>PBOADA@UCI.EDU</t>
+  </si>
+  <si>
+    <t>MCSB</t>
+  </si>
+  <si>
+    <t>G6</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>DA SILVA, KATE</t>
+  </si>
+  <si>
+    <t>KDASILV1@UCI.EDU</t>
+  </si>
+  <si>
+    <t>DALVI, ASHISH SENA</t>
+  </si>
+  <si>
+    <t>ASDALVI@UCI.EDU</t>
+  </si>
+  <si>
+    <t>DASH, AKARSH KUMAR</t>
+  </si>
+  <si>
+    <t>AKDASH@UCI.EDU</t>
+  </si>
+  <si>
+    <t>ESPELETA, ANA</t>
+  </si>
+  <si>
+    <t>AESPELET@UCI.EDU</t>
+  </si>
+  <si>
+    <t>GORGI, MELIKA</t>
+  </si>
+  <si>
+    <t>MGORGI@UCI.EDU</t>
+  </si>
+  <si>
+    <t>HENDRICK, CALEB WILSON</t>
+  </si>
+  <si>
+    <t>CWHENDRI@UCI.EDU</t>
+  </si>
+  <si>
+    <t>LEE, SINAI</t>
+  </si>
+  <si>
+    <t>SINAIL@UCI.EDU</t>
+  </si>
+  <si>
+    <t>LO, SHING</t>
+  </si>
+  <si>
+    <t>SHINGL2@UCI.EDU</t>
+  </si>
+  <si>
+    <t>NGUYEN, CHELSEA</t>
+  </si>
+  <si>
+    <t>CHELSEBN@UCI.EDU</t>
+  </si>
+  <si>
+    <t>PRABHAKAR, GAUTHAM</t>
+  </si>
+  <si>
+    <t>PRABHAKG@UCI.EDU</t>
+  </si>
+  <si>
+    <t>SAWA, YUN CHENG</t>
+  </si>
+  <si>
+    <t>YCSAWA@UCI.EDU</t>
+  </si>
+  <si>
+    <t>WANG, ETHAN</t>
+  </si>
+  <si>
+    <t>ETHAW13@UCI.EDU</t>
+  </si>
+  <si>
+    <t>G5</t>
+  </si>
+  <si>
+    <t>Ashish</t>
+  </si>
+  <si>
+    <t>Akarsh</t>
+  </si>
+  <si>
+    <t>Ana</t>
+  </si>
+  <si>
+    <t>Melika</t>
+  </si>
+  <si>
+    <t>Caleb</t>
+  </si>
+  <si>
+    <t>Sinai</t>
+  </si>
+  <si>
+    <t>Shing</t>
+  </si>
+  <si>
+    <t>Chelsea</t>
+  </si>
+  <si>
+    <t>Gautham</t>
+  </si>
+  <si>
+    <t>Yun</t>
+  </si>
+  <si>
+    <t>Ethan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -154,9 +223,26 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Times"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Times"/>
     </font>
   </fonts>
   <fills count="2">
@@ -180,12 +266,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -205,9 +295,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -245,7 +335,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -351,7 +441,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -493,7 +583,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -501,192 +591,368 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB30F65-A83E-A445-BF53-0C354A2986B1}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="29.83203125" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="G1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="C2" s="8">
+        <v>12869306</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="C3" s="8">
+        <v>77258971</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="F3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="8">
+        <v>43828638</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="F4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="8">
+        <v>15966282</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="8">
+        <v>48248275</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="8">
+        <v>23129348</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="8">
+        <v>36126466</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="8">
+        <v>75974441</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="8">
+        <v>73798823</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="8">
+        <v>30249449</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="8">
+        <v>50122326</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="8"/>
+    </row>
+    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="8">
+        <v>10443314</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="8">
+        <v>33689885</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="8"/>
+    </row>
+    <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B15" s="6"/>
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="1"/>
+    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B16" s="6"/>
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
       <c r="E16" s="1"/>
@@ -694,10 +960,7 @@
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="6"/>
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
       <c r="E17" s="1"/>
@@ -705,10 +968,7 @@
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
       <c r="E18" s="1"/>
@@ -716,31 +976,46 @@
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>27</v>
-      </c>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="A21" s="3"/>
+      <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>25</v>
-      </c>
+      <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>26</v>
-      </c>
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="mailto:PBOADA@UCI.EDU" xr:uid="{C158F58D-D4A9-C747-88F7-7F3F5A519200}"/>
+    <hyperlink ref="E3" r:id="rId2" display="mailto:KDASILV1@UCI.EDU" xr:uid="{F3E20449-3D8C-274E-B204-EC965E92C910}"/>
+    <hyperlink ref="E4" r:id="rId3" display="mailto:ASDALVI@UCI.EDU" xr:uid="{635F8998-134F-4344-80AE-5772EEB9BB69}"/>
+    <hyperlink ref="E5" r:id="rId4" display="mailto:AKDASH@UCI.EDU" xr:uid="{DA60AFD8-86B0-2145-B03C-851927E4E168}"/>
+    <hyperlink ref="E6" r:id="rId5" display="mailto:AESPELET@UCI.EDU" xr:uid="{A06568C3-93AA-BB45-819F-15B388CCF7DC}"/>
+    <hyperlink ref="E7" r:id="rId6" display="mailto:MGORGI@UCI.EDU" xr:uid="{59ECBC30-365E-E74B-949C-A2F7D4A2A1FD}"/>
+    <hyperlink ref="E8" r:id="rId7" display="mailto:CWHENDRI@UCI.EDU" xr:uid="{15FE4870-ABC7-6B4F-8381-1844CDFFDCE5}"/>
+    <hyperlink ref="E9" r:id="rId8" display="mailto:SINAIL@UCI.EDU" xr:uid="{852ED8C6-D1B6-1C45-B5BF-60DD8EEB883D}"/>
+    <hyperlink ref="E10" r:id="rId9" display="mailto:SHINGL2@UCI.EDU" xr:uid="{C87F0B5E-7A2A-0A43-A5AA-3EFE77C9ABF1}"/>
+    <hyperlink ref="E11" r:id="rId10" display="mailto:CHELSEBN@UCI.EDU" xr:uid="{601CAFF2-FE34-B943-B92A-04895BAC3937}"/>
+    <hyperlink ref="E12" r:id="rId11" display="mailto:PRABHAKG@UCI.EDU" xr:uid="{2A884390-2527-7E47-8C80-331EED3C8E31}"/>
+    <hyperlink ref="E13" r:id="rId12" display="mailto:YCSAWA@UCI.EDU" xr:uid="{56A2BB3C-3CF6-C343-8F07-F664DE1CA10D}"/>
+    <hyperlink ref="E14" r:id="rId13" display="mailto:ETHAW13@UCI.EDU" xr:uid="{00EE8B47-E2EF-A64D-8701-041D9403F3D8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>